<commit_message>
Test v0.99.1 1-14-21 Corsair
</commit_message>
<xml_diff>
--- a/NVIDIA RLA Mice Database - Github.xlsx
+++ b/NVIDIA RLA Mice Database - Github.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Reflex-Latency-Analyzer-Mouse-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2FA0A6-F106-4B7B-A72C-522C633637A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5F04FE-F62B-461E-A4E9-10EC4510D487}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4965" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LUT DB Public" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LUT DB Public'!$A$1:$Q$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LUT DB Public'!$A$1:$Q$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="288">
   <si>
     <t>Tested By</t>
   </si>
@@ -876,7 +876,28 @@
     <t>10781</t>
   </si>
   <si>
-    <t>v0.99.0 1-11-21</t>
+    <t>v0.99.1 1-14-21</t>
+  </si>
+  <si>
+    <t>Corsair</t>
+  </si>
+  <si>
+    <t>Dark Core rgb PRO SE (wireless)</t>
+  </si>
+  <si>
+    <t>1b1c</t>
+  </si>
+  <si>
+    <t>1b7f</t>
+  </si>
+  <si>
+    <t>0800</t>
+  </si>
+  <si>
+    <t>1207</t>
+  </si>
+  <si>
+    <t>329</t>
   </si>
 </sst>
 </file>
@@ -962,59 +983,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0E0E3"/>
-          <bgColor rgb="FFD0E0E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0E0E3"/>
-          <bgColor rgb="FFD0E0E3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1257,14 +1230,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1438,7 +1411,7 @@
         <v>32</v>
       </c>
       <c r="P3" s="5" t="str">
-        <f t="shared" ref="P3:P60" si="0">IF(K3 = 0,N3,((1000*(K3/M3) - L3)/2) +N3)</f>
+        <f t="shared" ref="P3:P61" si="0">IF(K3 = 0,N3,((1000*(K3/M3) - L3)/2) +N3)</f>
         <v>2115</v>
       </c>
       <c r="Q3" s="5" t="s">
@@ -1663,37 +1636,37 @@
     </row>
     <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>58</v>
+        <v>281</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>59</v>
+        <v>282</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>60</v>
+        <v>283</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>61</v>
+        <v>284</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>62</v>
+        <v>285</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>0</v>
+      <c r="H8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>24</v>
@@ -1702,14 +1675,13 @@
         <v>30</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>63</v>
+        <v>286</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="P8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>6132</v>
+        <v>287</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>286</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>1</v>
@@ -1720,7 +1692,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>60</v>
@@ -1756,14 +1728,14 @@
         <v>30</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>6164</v>
+        <v>6132</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>1</v>
@@ -1774,7 +1746,7 @@
         <v>58</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>60</v>
@@ -1810,14 +1782,14 @@
         <v>30</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>6330</v>
+        <v>6164</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>1</v>
@@ -1828,7 +1800,7 @@
         <v>58</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>60</v>
@@ -1864,14 +1836,14 @@
         <v>30</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P11" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>6595</v>
+        <v>6330</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>1</v>
@@ -1879,16 +1851,16 @@
     </row>
     <row r="12" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>62</v>
@@ -1918,14 +1890,14 @@
         <v>30</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>13461</v>
+        <v>6595</v>
       </c>
       <c r="Q12" s="5" t="s">
         <v>1</v>
@@ -1933,19 +1905,19 @@
     </row>
     <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>22</v>
@@ -1972,14 +1944,14 @@
         <v>30</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="P13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>8380</v>
+        <v>13461</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>1</v>
@@ -1987,19 +1959,19 @@
     </row>
     <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>22</v>
@@ -2026,14 +1998,14 @@
         <v>30</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="P14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2497</v>
+        <v>8380</v>
       </c>
       <c r="Q14" s="5" t="s">
         <v>1</v>
@@ -2044,16 +2016,16 @@
         <v>87</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>22</v>
@@ -2061,11 +2033,11 @@
       <c r="G15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>50</v>
+      <c r="H15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="J15" s="5" t="b">
         <v>0</v>
@@ -2080,14 +2052,14 @@
         <v>30</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="P15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2562</v>
+        <v>2497</v>
       </c>
       <c r="Q15" s="5" t="s">
         <v>1</v>
@@ -2107,7 +2079,7 @@
         <v>95</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>22</v>
@@ -2118,8 +2090,8 @@
       <c r="H16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="5" t="b">
-        <v>1</v>
+      <c r="I16" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="J16" s="5" t="b">
         <v>0</v>
@@ -2134,14 +2106,14 @@
         <v>30</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2523</v>
+        <v>2562</v>
       </c>
       <c r="Q16" s="5" t="s">
         <v>1</v>
@@ -2151,8 +2123,8 @@
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>102</v>
+      <c r="B17" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>89</v>
@@ -2161,7 +2133,7 @@
         <v>95</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>22</v>
@@ -2172,8 +2144,8 @@
       <c r="H17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>50</v>
+      <c r="I17" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="J17" s="5" t="b">
         <v>0</v>
@@ -2188,14 +2160,14 @@
         <v>30</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>1</v>
@@ -2215,7 +2187,7 @@
         <v>95</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>22</v>
@@ -2227,7 +2199,7 @@
         <v>50</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="J18" s="5" t="b">
         <v>0</v>
@@ -2242,14 +2214,14 @@
         <v>30</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>1</v>
@@ -2259,8 +2231,8 @@
       <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>107</v>
+      <c r="B19" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>89</v>
@@ -2269,7 +2241,7 @@
         <v>95</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>22</v>
@@ -2281,7 +2253,7 @@
         <v>50</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="J19" s="5" t="b">
         <v>0</v>
@@ -2296,14 +2268,14 @@
         <v>30</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P19" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2553</v>
+        <v>2529</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>1</v>
@@ -2323,7 +2295,7 @@
         <v>95</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>22</v>
@@ -2335,7 +2307,7 @@
         <v>50</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="J20" s="5" t="b">
         <v>0</v>
@@ -2350,14 +2322,14 @@
         <v>30</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P20" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2537</v>
+        <v>2553</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>1</v>
@@ -2368,16 +2340,16 @@
         <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>22</v>
@@ -2385,11 +2357,11 @@
       <c r="G21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5" t="b">
-        <v>0</v>
+      <c r="H21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="J21" s="5" t="b">
         <v>0</v>
@@ -2404,14 +2376,14 @@
         <v>30</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="P21" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>3025</v>
+        <v>2537</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>1</v>
@@ -2428,10 +2400,10 @@
         <v>89</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>22</v>
@@ -2458,14 +2430,14 @@
         <v>30</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="P22" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2554</v>
+        <v>3025</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>1</v>
@@ -2476,16 +2448,16 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>22</v>
@@ -2512,14 +2484,14 @@
         <v>30</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="P23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2809</v>
+        <v>2554</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>1</v>
@@ -2530,16 +2502,16 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>22</v>
@@ -2566,14 +2538,14 @@
         <v>30</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="P24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2919</v>
+        <v>2809</v>
       </c>
       <c r="Q24" s="5" t="s">
         <v>1</v>
@@ -2584,16 +2556,16 @@
         <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>22</v>
@@ -2620,14 +2592,14 @@
         <v>30</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>3179</v>
+        <v>2919</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>1</v>
@@ -2638,158 +2610,158 @@
         <v>87</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="P26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>3179</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" s="6">
-        <v>0</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N26" s="5" t="s">
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="6">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="O26" s="5" t="s">
+      <c r="O27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="P26" s="5" t="str">
+      <c r="P27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2537</v>
       </c>
-      <c r="Q26" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="Q27" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E28" s="6">
         <v>4501</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K27" s="6">
-        <v>0</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" s="6">
+      <c r="F28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="6">
         <v>1000</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N28" s="6">
         <v>2562</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O28" s="6">
         <v>291</v>
       </c>
-      <c r="P27" s="5">
+      <c r="P28" s="5">
         <f t="shared" si="0"/>
         <v>2562</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K28" s="6">
-        <v>0</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="P28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>2516</v>
       </c>
       <c r="Q28" s="5" t="s">
         <v>1</v>
@@ -2800,16 +2772,16 @@
         <v>87</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>22</v>
@@ -2836,14 +2808,14 @@
         <v>30</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="P29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>2527</v>
+        <v>2516</v>
       </c>
       <c r="Q29" s="5" t="s">
         <v>1</v>
@@ -2853,26 +2825,26 @@
       <c r="A30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>152</v>
+      <c r="B30" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>50</v>
@@ -2880,8 +2852,8 @@
       <c r="J30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>24</v>
+      <c r="K30" s="6">
+        <v>0</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>24</v>
@@ -2890,14 +2862,14 @@
         <v>30</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="P30" s="7">
-        <f t="shared" si="0"/>
-        <v>1843</v>
+        <v>151</v>
+      </c>
+      <c r="P30" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>2527</v>
       </c>
       <c r="Q30" s="5" t="s">
         <v>1</v>
@@ -2908,105 +2880,106 @@
         <v>87</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="P31" s="7">
+        <f t="shared" si="0"/>
+        <v>1843</v>
+      </c>
+      <c r="Q31" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="5" t="s">
+      <c r="F32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N31" s="8" t="s">
+      <c r="J32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="O31" s="5" t="s">
+      <c r="O32" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="P31" s="7">
+      <c r="P32" s="7">
         <f t="shared" si="0"/>
         <v>808</v>
       </c>
-      <c r="Q31" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N32" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P32" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q32" s="10" t="s">
+      <c r="Q32" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3015,16 +2988,16 @@
         <v>258</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>260</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>62</v>
+        <v>270</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>22</v>
@@ -3051,13 +3024,13 @@
         <v>30</v>
       </c>
       <c r="N33" s="11" t="s">
-        <v>272</v>
+        <v>205</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P33" s="13" t="s">
-        <v>272</v>
+        <v>205</v>
       </c>
       <c r="Q33" s="10" t="s">
         <v>1</v>
@@ -3068,16 +3041,16 @@
         <v>258</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>260</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>274</v>
+        <v>62</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>22</v>
@@ -3104,13 +3077,13 @@
         <v>30</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>86</v>
+        <v>273</v>
       </c>
       <c r="P34" s="13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="Q34" s="10" t="s">
         <v>1</v>
@@ -3121,16 +3094,16 @@
         <v>258</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>260</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>22</v>
@@ -3157,13 +3130,13 @@
         <v>30</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>278</v>
+        <v>86</v>
       </c>
       <c r="P35" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q35" s="10" t="s">
         <v>1</v>
@@ -3174,105 +3147,104 @@
         <v>258</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>260</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="P36" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q36" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N36" s="11" t="s">
+      <c r="F37" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N37" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="O36" s="10" t="s">
+      <c r="O37" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="P36" s="13" t="s">
+      <c r="P37" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="Q36" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" s="6">
-        <v>0</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="P37" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-      <c r="Q37" s="5" t="s">
+      <c r="Q37" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3281,19 +3253,19 @@
         <v>161</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>23</v>
@@ -3317,14 +3289,14 @@
         <v>30</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="P38" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>1587</v>
+        <v>1400</v>
       </c>
       <c r="Q38" s="5" t="s">
         <v>1</v>
@@ -3335,19 +3307,19 @@
         <v>161</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
@@ -3355,11 +3327,11 @@
       <c r="H39" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" s="5" t="b">
-        <v>0</v>
+      <c r="I39" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="K39" s="6">
         <v>0</v>
@@ -3371,14 +3343,14 @@
         <v>30</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="P39" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10150</v>
+        <v>1587</v>
       </c>
       <c r="Q39" s="5" t="s">
         <v>1</v>
@@ -3389,13 +3361,13 @@
         <v>161</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>172</v>
@@ -3409,30 +3381,30 @@
       <c r="H40" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>50</v>
+      <c r="I40" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="J40" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="6">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>177</v>
+        <v>24</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>30</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="P40" s="5">
-        <f t="shared" si="0"/>
-        <v>2234</v>
+        <v>174</v>
+      </c>
+      <c r="P40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>10150</v>
       </c>
       <c r="Q40" s="5" t="s">
         <v>1</v>
@@ -3443,16 +3415,16 @@
         <v>161</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>62</v>
+        <v>172</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>22</v>
@@ -3463,17 +3435,17 @@
       <c r="H41" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="5" t="b">
-        <v>0</v>
+      <c r="I41" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="J41" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K41" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>30</v>
@@ -3482,11 +3454,11 @@
         <v>178</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>116</v>
+        <v>179</v>
       </c>
       <c r="P41" s="5">
         <f t="shared" si="0"/>
-        <v>1719</v>
+        <v>2234</v>
       </c>
       <c r="Q41" s="5" t="s">
         <v>1</v>
@@ -3497,19 +3469,19 @@
         <v>161</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>23</v>
@@ -3533,14 +3505,14 @@
         <v>30</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
       <c r="P42" s="5">
         <f t="shared" si="0"/>
-        <v>2517</v>
+        <v>1719</v>
       </c>
       <c r="Q42" s="5" t="s">
         <v>1</v>
@@ -3548,22 +3520,22 @@
     </row>
     <row r="43" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
@@ -3572,29 +3544,29 @@
         <v>0</v>
       </c>
       <c r="I43" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="6">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>24</v>
+        <v>182</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>30</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="P43" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>3108</v>
+        <v>186</v>
+      </c>
+      <c r="P43" s="5">
+        <f t="shared" si="0"/>
+        <v>2517</v>
       </c>
       <c r="Q43" s="5" t="s">
         <v>1</v>
@@ -3611,10 +3583,10 @@
         <v>189</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>22</v>
@@ -3622,14 +3594,14 @@
       <c r="G44" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H44" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>50</v>
+      <c r="H44" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="K44" s="6">
         <v>0</v>
@@ -3641,14 +3613,14 @@
         <v>30</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="P44" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>5123</v>
+        <v>3108</v>
       </c>
       <c r="Q44" s="5" t="s">
         <v>1</v>
@@ -3656,19 +3628,19 @@
     </row>
     <row r="45" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>189</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>22</v>
@@ -3676,14 +3648,14 @@
       <c r="G45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" s="5" t="b">
-        <v>0</v>
+      <c r="H45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="K45" s="6">
         <v>0</v>
@@ -3695,14 +3667,14 @@
         <v>30</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="P45" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>8542</v>
+        <v>5123</v>
       </c>
       <c r="Q45" s="5" t="s">
         <v>1</v>
@@ -3710,19 +3682,19 @@
     </row>
     <row r="46" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>189</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>22</v>
@@ -3749,14 +3721,14 @@
         <v>30</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P46" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>8790</v>
+        <v>8542</v>
       </c>
       <c r="Q46" s="5" t="s">
         <v>1</v>
@@ -3764,19 +3736,19 @@
     </row>
     <row r="47" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>2</v>
+        <v>187</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>22</v>
@@ -3803,14 +3775,14 @@
         <v>30</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P47" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10067</v>
+        <v>8790</v>
       </c>
       <c r="Q47" s="5" t="s">
         <v>1</v>
@@ -3821,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>210</v>
@@ -3857,14 +3829,14 @@
         <v>30</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P48" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10076</v>
+        <v>10067</v>
       </c>
       <c r="Q48" s="5" t="s">
         <v>1</v>
@@ -3875,7 +3847,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>210</v>
@@ -3911,14 +3883,14 @@
         <v>30</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="P49" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10205</v>
+        <v>10076</v>
       </c>
       <c r="Q49" s="5" t="s">
         <v>1</v>
@@ -3929,7 +3901,7 @@
         <v>2</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>210</v>
@@ -3965,14 +3937,14 @@
         <v>30</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P50" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10209</v>
+        <v>10205</v>
       </c>
       <c r="Q50" s="5" t="s">
         <v>1</v>
@@ -3983,7 +3955,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>210</v>
@@ -4019,14 +3991,14 @@
         <v>30</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P51" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10306</v>
+        <v>10209</v>
       </c>
       <c r="Q51" s="5" t="s">
         <v>1</v>
@@ -4037,7 +4009,7 @@
         <v>2</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>210</v>
@@ -4073,14 +4045,14 @@
         <v>30</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="P52" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10362</v>
+        <v>10306</v>
       </c>
       <c r="Q52" s="5" t="s">
         <v>1</v>
@@ -4091,7 +4063,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>210</v>
@@ -4127,14 +4099,14 @@
         <v>30</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P53" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>10364</v>
+        <v>10362</v>
       </c>
       <c r="Q53" s="5" t="s">
         <v>1</v>
@@ -4145,16 +4117,16 @@
         <v>2</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>22</v>
@@ -4181,14 +4153,14 @@
         <v>30</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="P54" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>7237</v>
+        <v>10364</v>
       </c>
       <c r="Q54" s="5" t="s">
         <v>1</v>
@@ -4199,7 +4171,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>233</v>
@@ -4235,14 +4207,14 @@
         <v>30</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="P55" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>7241</v>
+        <v>7237</v>
       </c>
       <c r="Q55" s="5" t="s">
         <v>1</v>
@@ -4253,7 +4225,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>233</v>
@@ -4289,14 +4261,14 @@
         <v>30</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="P56" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>7297</v>
+        <v>7241</v>
       </c>
       <c r="Q56" s="5" t="s">
         <v>1</v>
@@ -4307,7 +4279,7 @@
         <v>2</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>233</v>
@@ -4343,14 +4315,14 @@
         <v>30</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O57" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="P57" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>7316</v>
+        <v>7297</v>
       </c>
       <c r="Q57" s="5" t="s">
         <v>1</v>
@@ -4361,16 +4333,16 @@
         <v>2</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>22</v>
@@ -4397,14 +4369,14 @@
         <v>30</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O58" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="P58" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>7401</v>
+        <v>7316</v>
       </c>
       <c r="Q58" s="5" t="s">
         <v>1</v>
@@ -4415,16 +4387,16 @@
         <v>2</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>252</v>
+        <v>211</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>22</v>
@@ -4451,14 +4423,14 @@
         <v>30</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="P59" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>7623</v>
+        <v>7401</v>
       </c>
       <c r="Q59" s="5" t="s">
         <v>1</v>
@@ -4469,69 +4441,123 @@
         <v>2</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" s="6">
+        <v>0</v>
+      </c>
+      <c r="L60" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N60" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="O60" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="P60" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>7623</v>
+      </c>
+      <c r="Q60" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E61" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="F60" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K60" s="6">
-        <v>0</v>
-      </c>
-      <c r="L60" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N60" s="5" t="s">
+      <c r="F61" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" s="6">
+        <v>0</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N61" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="O60" s="5" t="s">
+      <c r="O61" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="P60" s="5" t="str">
+      <c r="P61" s="5" t="str">
         <f t="shared" si="0"/>
         <v>7658</v>
       </c>
-      <c r="Q60" s="5" t="s">
+      <c r="Q61" s="5" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q60" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="G31:G36">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="true">
-      <formula>NOT(ISERROR(SEARCH(("true"),(H31))))</formula>
+  <autoFilter ref="A1:Q61" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <conditionalFormatting sqref="G32:G37">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="true">
+      <formula>NOT(ISERROR(SEARCH(("true"),(H32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I26 I28:I60">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="true">
+  <conditionalFormatting sqref="I1:I27 I29:I61">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="true">
       <formula>NOT(ISERROR(SEARCH(("true"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26 J28:J60">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="J2:J27 J29:J61">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH(("TRUE"),(J2))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>